<commit_message>
started analysis of spok and various kernels
</commit_message>
<xml_diff>
--- a/results_analysis/spark_wallFollow_01_hold_02.xlsx
+++ b/results_analysis/spark_wallFollow_01_hold_02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4FC28B-155E-49A5-A917-68A4F199D6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA545D6-439B-4675-A44E-B678B04828AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -807,7 +807,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -823,24 +841,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,48 +1146,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="68"/>
-      <c r="M3" s="66" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="66"/>
+      <c r="M3" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="68"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="66"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1328,7 +1328,7 @@
         <f t="shared" si="0"/>
         <v>-0.32233480176211404</v>
       </c>
-      <c r="W5" s="69">
+      <c r="W5" s="60">
         <f t="shared" si="0"/>
         <v>-4.0903083700440046E-2</v>
       </c>
@@ -1395,7 +1395,7 @@
         <f t="shared" si="0"/>
         <v>-0.42898678414096902</v>
       </c>
-      <c r="W6" s="70">
+      <c r="W6" s="61">
         <f t="shared" si="0"/>
         <v>-4.4449339207048966E-2</v>
       </c>
@@ -1467,7 +1467,7 @@
         <f t="shared" si="0"/>
         <v>-0.125859030837004</v>
       </c>
-      <c r="W7" s="70">
+      <c r="W7" s="61">
         <f t="shared" si="0"/>
         <v>-6.0572687224670352E-3</v>
       </c>
@@ -1535,7 +1535,7 @@
         <f t="shared" si="0"/>
         <v>-0.14066079295154199</v>
       </c>
-      <c r="W8" s="71">
+      <c r="W8" s="62">
         <f t="shared" si="0"/>
         <v>-3.9030837004405017E-2</v>
       </c>
@@ -1611,7 +1611,7 @@
         <f t="shared" si="1"/>
         <v>-8.8766519823789691E-3</v>
       </c>
-      <c r="W9" s="69">
+      <c r="W9" s="60">
         <f t="shared" si="1"/>
         <v>-3.6960352422907072E-2</v>
       </c>
@@ -1678,7 +1678,7 @@
         <f t="shared" si="1"/>
         <v>-8.6189427312775013E-2</v>
       </c>
-      <c r="W10" s="70">
+      <c r="W10" s="61">
         <f t="shared" si="1"/>
         <v>-2.9449339207048952E-2</v>
       </c>
@@ -1750,7 +1750,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W11" s="70">
+      <c r="W11" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1818,7 +1818,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W12" s="71">
+      <c r="W12" s="62">
         <f t="shared" si="1"/>
         <v>-3.1938325991189842E-3</v>
       </c>
@@ -1894,7 +1894,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W13" s="69">
+      <c r="W13" s="60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1961,7 +1961,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W14" s="70">
+      <c r="W14" s="61">
         <f t="shared" si="2"/>
         <v>-4.4493392070490412E-3</v>
       </c>
@@ -2033,7 +2033,7 @@
         <f t="shared" si="2"/>
         <v>-0.31931718061673997</v>
       </c>
-      <c r="W15" s="70">
+      <c r="W15" s="61">
         <f t="shared" si="2"/>
         <v>-0.3326872246696041</v>
       </c>
@@ -2101,7 +2101,7 @@
         <f t="shared" si="2"/>
         <v>-0.35207048458149803</v>
       </c>
-      <c r="W16" s="71">
+      <c r="W16" s="62">
         <f t="shared" si="2"/>
         <v>-0.27861233480176195</v>
       </c>
@@ -2177,7 +2177,7 @@
         <f t="shared" si="3"/>
         <v>-0.34555066079295205</v>
       </c>
-      <c r="W17" s="69">
+      <c r="W17" s="60">
         <f t="shared" si="3"/>
         <v>-4.8656387665198086E-2</v>
       </c>
@@ -2244,7 +2244,7 @@
         <f t="shared" si="3"/>
         <v>-0.23482378854625607</v>
       </c>
-      <c r="W18" s="70">
+      <c r="W18" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2316,7 +2316,7 @@
         <f t="shared" si="3"/>
         <v>-6.1762114537444956E-2</v>
       </c>
-      <c r="W19" s="70">
+      <c r="W19" s="61">
         <f t="shared" si="3"/>
         <v>-6.7621145374450187E-3</v>
       </c>
@@ -2384,7 +2384,7 @@
         <f t="shared" si="3"/>
         <v>-0.13233480176211498</v>
       </c>
-      <c r="W20" s="71">
+      <c r="W20" s="62">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2400,32 +2400,32 @@
       <c r="K21" s="16"/>
     </row>
     <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="68"/>
-      <c r="M22" s="66" t="s">
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="66"/>
+      <c r="M22" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="N22" s="67"/>
-      <c r="O22" s="67"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="67"/>
-      <c r="T22" s="67"/>
-      <c r="U22" s="67"/>
-      <c r="V22" s="67"/>
-      <c r="W22" s="68"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="65"/>
+      <c r="R22" s="65"/>
+      <c r="S22" s="65"/>
+      <c r="T22" s="65"/>
+      <c r="U22" s="65"/>
+      <c r="V22" s="65"/>
+      <c r="W22" s="66"/>
     </row>
     <row r="23" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -3930,61 +3930,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="62" t="s">
+      <c r="E3" s="69"/>
+      <c r="F3" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="62" t="s">
+      <c r="G3" s="69"/>
+      <c r="H3" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="62" t="s">
+      <c r="I3" s="69"/>
+      <c r="J3" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="63"/>
-      <c r="L3" s="62" t="s">
+      <c r="K3" s="69"/>
+      <c r="L3" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="63"/>
-      <c r="N3" s="62" t="s">
+      <c r="M3" s="69"/>
+      <c r="N3" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="63"/>
-      <c r="P3" s="62" t="s">
+      <c r="O3" s="69"/>
+      <c r="P3" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="62" t="s">
+      <c r="Q3" s="69"/>
+      <c r="R3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="64"/>
+      <c r="S3" s="70"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -5269,19 +5269,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -5872,19 +5872,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -6463,8 +6463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4FABDC-54DB-4F0C-8A5E-619A5BBC4590}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6482,19 +6482,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7082,7 +7082,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
+      <c r="F24" s="1"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
@@ -7410,19 +7410,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8180,19 +8180,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9108,19 +9108,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9878,19 +9878,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10648,19 +10648,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11418,19 +11418,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12190,24 +12190,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12217,29 +12217,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="62" t="s">
+      <c r="K3" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="62" t="s">
+      <c r="L3" s="69"/>
+      <c r="M3" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="62" t="s">
+      <c r="N3" s="69"/>
+      <c r="O3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="64"/>
+      <c r="P3" s="70"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">

</xml_diff>